<commit_message>
added new api method
</commit_message>
<xml_diff>
--- a/src/test/resources/Report.xlsx
+++ b/src/test/resources/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -48,12 +48,510 @@
   </si>
   <si>
     <t>ResponseTime</t>
+  </si>
+  <si>
+    <t>Tc002</t>
+  </si>
+  <si>
+    <t>Get request testing</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.comcommentspostId=1</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "postId": 1,
+        "id": 1,
+        "name": "id labore ex et quam laborum",
+        "email": "Eliseo@gardner.biz",
+        "body": "laudantium enim quasi est quidem magnam voluptate ipsam eos\ntempora quo necessitatibus\ndolor quam autem quasi\nreiciendis et nam sapiente accusantium"
+    },
+    {
+        "postId": 1,
+        "id": 2,
+        "name": "quo vero reiciendis velit similique earum",
+        "email": "Jayne_Kuhic@sydney.com",
+        "body": "est natus enim nihil est dolore omnis voluptatem numquam\net omnis occaecati quod ullam at\nvoluptatem error expedita pariatur\nnihil sint nostrum voluptatem reiciendis et"
+    },
+    {
+        "postId": 1,
+        "id": 3,
+        "name": "odio adipisci rerum aut animi",
+        "email": "Nikita@garfield.biz",
+        "body": "quia molestiae reprehenderit quasi aspernatur\naut expedita occaecati aliquam eveniet laudantium\nomnis quibusdam delectus saepe quia accusamus maiores nam est\ncum et ducimus et vero voluptates excepturi deleniti ratione"
+    },
+    {
+        "postId": 1,
+        "id": 4,
+        "name": "alias odio sit",
+        "email": "Lew@alysha.tv",
+        "body": "non et atque\noccaecati deserunt quas accusantium unde odit nobis qui voluptatem\nquia voluptas consequuntur itaque dolor\net qui rerum deleniti ut occaecati"
+    },
+    {
+        "postId": 1,
+        "id": 5,
+        "name": "vero eaque aliquid doloribus et culpa",
+        "email": "Hayden@althea.biz",
+        "body": "harum non quasi et ratione\ntempore iure ex voluptates in ratione\nharum architecto fugit inventore cupiditate\nvoluptates magni quo et"
+    }
+]</t>
+  </si>
+  <si>
+    <t>Date=Sun, 22 Jun 2025 13:38:19 GMT
+Content-Type=application/json; charset=utf-8
+Content-Length=657
+Connection=keep-alive
+Access-Control-Allow-Credentials=true
+Cache-Control=max-age=43200
+Content-Encoding=gzip
+Etag=W/"5e6-4bSPS5tq8F8ZDeFJULWh6upjp7U"
+Expires=-1
+Nel={"report_to":"heroku-nel","response_headers":["Via"],"max_age":3600,"success_fraction":0.01,"failure_fraction":0.1}
+Pragma=no-cache
+Report-To={"group":"heroku-nel","endpoints":[{"url":"https://nel.heroku.com/reports?s=QBhyummfvQJGH9ambSlADZ0AEU3JxvfQG8IZSPIADG4%3D\u0026sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d\u0026ts=1749055630"}],"max_age":3600}
+Reporting-Endpoints=heroku-nel="https://nel.heroku.com/reports?s=QBhyummfvQJGH9ambSlADZ0AEU3JxvfQG8IZSPIADG4%3D&amp;sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d&amp;ts=1749055630"
+Server=cloudflare
+Vary=Origin, Accept-Encoding
+Via=2.0 heroku-router
+X-Content-Type-Options=nosniff
+X-Powered-By=Express
+X-Ratelimit-Limit=1000
+X-Ratelimit-Remaining=999
+X-Ratelimit-Reset=1749055651
+Age=15482
+Cf-Cache-Status=HIT
+CF-RAY=953c25393c825d7c-FRA
+alt-svc=h3=":443"; ma=86400</t>
+  </si>
+  <si>
+    <t>1591</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tc001</t>
+  </si>
+  <si>
+    <t>Get Request testing</t>
+  </si>
+  <si>
+    <t>https://dummyjson.comusers</t>
+  </si>
+  <si>
+    <t>Content exceeds max cell length.... see data in logs</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Sun, 22 Jun 2025 13:38:19 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=Ig23NYTeQKWC_dgNDcO5xA
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1750599500
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1561</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Mon, 23 Jun 2025 07:28:31 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=uY7-i3yDQJy34ApCDcO5xA
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1750663716
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1735</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Mon, 23 Jun 2025 07:35:53 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=PC3XJzTuS9Cp3rdlDcO5xA
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1750664157
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1570</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Mon, 23 Jun 2025 07:38:00 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=co3zVSNmSW-b3uGRAQeqjw
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1750664286
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1678</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Mon, 23 Jun 2025 07:39:14 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=hl5jL76eQ2Szgbx_AQeqjw
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1750664356
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1681</t>
+  </si>
+  <si>
+    <t>Date=Mon, 23 Jun 2025 07:39:14 GMT
+Content-Type=application/json; charset=utf-8
+Content-Length=657
+Connection=keep-alive
+Access-Control-Allow-Credentials=true
+Cache-Control=max-age=43200
+Content-Encoding=gzip
+Etag=W/"5e6-4bSPS5tq8F8ZDeFJULWh6upjp7U"
+Expires=-1
+Nel={"report_to":"heroku-nel","response_headers":["Via"],"max_age":3600,"success_fraction":0.01,"failure_fraction":0.1}
+Pragma=no-cache
+Report-To={"group":"heroku-nel","endpoints":[{"url":"https://nel.heroku.com/reports?s=QBhyummfvQJGH9ambSlADZ0AEU3JxvfQG8IZSPIADG4%3D\u0026sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d\u0026ts=1749055630"}],"max_age":3600}
+Reporting-Endpoints=heroku-nel="https://nel.heroku.com/reports?s=QBhyummfvQJGH9ambSlADZ0AEU3JxvfQG8IZSPIADG4%3D&amp;sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d&amp;ts=1749055630"
+Server=cloudflare
+Vary=Origin, Accept-Encoding
+Via=2.0 heroku-router
+X-Content-Type-Options=nosniff
+X-Powered-By=Express
+X-Ratelimit-Limit=1000
+X-Ratelimit-Remaining=999
+X-Ratelimit-Reset=1749055651
+Age=9189
+Cf-Cache-Status=HIT
+CF-RAY=954254962d471d9a-FRA
+alt-svc=h3=":443"; ma=86400</t>
+  </si>
+  <si>
+    <t>1680</t>
+  </si>
+  <si>
+    <t>com.fasterxml.jackson.core.JsonParseException: Unexpected character ('t' (code 116)): was expecting comma to separate Object entries
+ at [Source: (StringReader); line: 1, column: 58]</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Wed, 25 Jun 2025 16:27:30 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=3rjWGMZ-TlSaHKBuacI7Nw
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1750868852
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1771</t>
+  </si>
+  <si>
+    <t>Date=Wed, 25 Jun 2025 16:27:30 GMT
+Content-Type=application/json; charset=utf-8
+Content-Length=657
+Connection=keep-alive
+Access-Control-Allow-Credentials=true
+Cache-Control=max-age=43200
+Content-Encoding=gzip
+Etag=W/"5e6-4bSPS5tq8F8ZDeFJULWh6upjp7U"
+Expires=-1
+Nel={"report_to":"heroku-nel","response_headers":["Via"],"max_age":3600,"success_fraction":0.01,"failure_fraction":0.1}
+Pragma=no-cache
+Report-To={"group":"heroku-nel","endpoints":[{"url":"https://nel.heroku.com/reports?s=QBhyummfvQJGH9ambSlADZ0AEU3JxvfQG8IZSPIADG4%3D\u0026sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d\u0026ts=1749055630"}],"max_age":3600}
+Reporting-Endpoints=heroku-nel="https://nel.heroku.com/reports?s=QBhyummfvQJGH9ambSlADZ0AEU3JxvfQG8IZSPIADG4%3D&amp;sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d&amp;ts=1749055630"
+Server=cloudflare
+Vary=Origin, Accept-Encoding
+Via=2.0 heroku-router
+X-Content-Type-Options=nosniff
+X-Powered-By=Express
+X-Ratelimit-Limit=1000
+X-Ratelimit-Remaining=999
+X-Ratelimit-Reset=1749055651
+Age=14148
+Cf-Cache-Status=HIT
+CF-RAY=9555d52bf80bdc90-FRA
+alt-svc=h3=":443"; ma=86400</t>
+  </si>
+  <si>
+    <t>1794</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Mon, 07 Jul 2025 06:59:07 GMT
+Etag=W/"a36f-Hyqmc+8fsEhjdF4H4imH3z/VXKo"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=mlYABKBYSm-ZNTegAQeqjw
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1751871554
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>Date=Mon, 07 Jul 2025 06:59:08 GMT
+Content-Type=application/json; charset=utf-8
+Transfer-Encoding=chunked
+Connection=keep-alive
+Access-Control-Allow-Credentials=true
+Cache-Control=max-age=43200
+Content-Encoding=gzip
+Etag=W/"5e6-4bSPS5tq8F8ZDeFJULWh6upjp7U"
+Expires=-1
+Nel={"report_to":"heroku-nel","response_headers":["Via"],"max_age":3600,"success_fraction":0.01,"failure_fraction":0.1}
+Pragma=no-cache
+Report-To={"group":"heroku-nel","endpoints":[{"url":"https://nel.heroku.com/reports?s=noZ47AufXY8moOcWlmFuXq8YMFa1Zsi%2BbJex5MJEYb0%3D\u0026sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d\u0026ts=1751731612"}],"max_age":3600}
+Reporting-Endpoints=heroku-nel="https://nel.heroku.com/reports?s=noZ47AufXY8moOcWlmFuXq8YMFa1Zsi%2BbJex5MJEYb0%3D&amp;sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d&amp;ts=1751731612"
+Server=cloudflare
+Vary=Origin, Accept-Encoding
+Via=2.0 heroku-router
+X-Content-Type-Options=nosniff
+X-Powered-By=Express
+X-Ratelimit-Limit=1000
+X-Ratelimit-Remaining=997
+X-Ratelimit-Reset=1751731648
+Cf-Cache-Status=REVALIDATED
+CF-RAY=95b57516aefd74e3-FRA
+alt-svc=h3=":443"; ma=86400</t>
+  </si>
+  <si>
+    <t>2044</t>
+  </si>
+  <si>
+    <t>https://dummyjson.comusers/1</t>
+  </si>
+  <si>
+    <t>{
+    "id": 1,
+    "firstName": "Emily",
+    "lastName": "Johnson",
+    "maidenName": "Smith",
+    "age": 28,
+    "gender": "female",
+    "email": "emily.johnson@x.dummyjson.com",
+    "phone": "+81 965-431-3024",
+    "username": "emilys",
+    "password": "emilyspass",
+    "birthDate": "1996-5-30",
+    "image": "https://dummyjson.com/icon/emilys/128",
+    "bloodGroup": "O-",
+    "height": 193.24,
+    "weight": 63.16,
+    "eyeColor": "Green",
+    "hair": {
+        "color": "Brown",
+        "type": "Curly"
+    },
+    "ip": "42.48.100.32",
+    "address": {
+        "address": "626 Main Street",
+        "city": "Phoenix",
+        "state": "Mississippi",
+        "stateCode": "MS",
+        "postalCode": "29112",
+        "coordinates": {
+            "lat": -77.16213,
+            "lng": -92.084824
+        },
+        "country": "United States"
+    },
+    "macAddress": "47:fa:41:18:ec:eb",
+    "university": "University of Wisconsin--Madison",
+    "bank": {
+        "cardExpire": "03/26",
+        "cardNumber": "9289760655481815",
+        "cardType": "Elo",
+        "currency": "CNY",
+        "iban": "YPUXISOBI7TTHPK2BR3HAIXL"
+    },
+    "company": {
+        "department": "Engineering",
+        "name": "Dooley, Kozey and Cronin",
+        "title": "Sales Manager",
+        "address": {
+            "address": "263 Tenth Street",
+            "city": "San Francisco",
+            "state": "Wisconsin",
+            "stateCode": "WI",
+            "postalCode": "37657",
+            "coordinates": {
+                "lat": 71.814525,
+                "lng": -161.150263
+            },
+            "country": "United States"
+        }
+    },
+    "ein": "977-175",
+    "ssn": "900-590-289",
+    "userAgent": "Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.93 Safari/537.36",
+    "crypto": {
+        "coin": "Bitcoin",
+        "wallet": "0xb9fc2fe63b2a6c003f1c324c3bfa53259162181a",
+        "network": "Ethereum (ERC20)"
+    },
+    "role": "admin"
+}</t>
+  </si>
+  <si>
+    <t>Access-Control-Allow-Origin=*
+Content-Encoding=gzip
+Content-Type=application/json; charset=utf-8
+Date=Mon, 07 Jul 2025 07:19:20 GMT
+Etag=W/"57b-eBF3JfwanM/U4Wy609CPdIf9zRA"
+Server=railway-edge
+Strict-Transport-Security=max-age=15552000; includeSubDomains
+Vary=Accept-Encoding
+X-Content-Type-Options=nosniff
+X-Dns-Prefetch-Control=off
+X-Download-Options=noopen
+X-Frame-Options=SAMEORIGIN
+X-Powered-By=Cats on Keyboards
+X-Railway-Edge=railway/asia-southeast1-eqsg3a
+X-Railway-Request-Id=kOd3GtdlTuaUaKnqAQeqjw
+X-Ratelimit-Limit=100
+X-Ratelimit-Remaining=99
+X-Ratelimit-Reset=1751872764
+X-Xss-Protection=1; mode=block
+Transfer-Encoding=chunked</t>
+  </si>
+  <si>
+    <t>1402</t>
+  </si>
+  <si>
+    <t>Date=Mon, 07 Jul 2025 07:19:20 GMT
+Content-Type=application/json; charset=utf-8
+Transfer-Encoding=chunked
+Connection=keep-alive
+Access-Control-Allow-Credentials=true
+Cache-Control=max-age=43200
+Content-Encoding=gzip
+Etag=W/"5e6-4bSPS5tq8F8ZDeFJULWh6upjp7U"
+Expires=-1
+Nel={"report_to":"heroku-nel","response_headers":["Via"],"max_age":3600,"success_fraction":0.01,"failure_fraction":0.1}
+Pragma=no-cache
+Report-To={"group":"heroku-nel","endpoints":[{"url":"https://nel.heroku.com/reports?s=PqH6pjE2xpV37bQoiBMDJaMTilWEqIjIYir6WsSpUFg%3D\u0026sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d\u0026ts=1751105391"}],"max_age":3600}
+Reporting-Endpoints=heroku-nel="https://nel.heroku.com/reports?s=PqH6pjE2xpV37bQoiBMDJaMTilWEqIjIYir6WsSpUFg%3D&amp;sid=e11707d5-02a7-43ef-b45e-2cf4d2036f7d&amp;ts=1751105391"
+Server=cloudflare
+Vary=Origin, Accept-Encoding
+Via=2.0 heroku-router
+X-Content-Type-Options=nosniff
+X-Powered-By=Express
+X-Ratelimit-Limit=1000
+X-Ratelimit-Remaining=999
+X-Ratelimit-Reset=1751105415
+Age=575
+Cf-Cache-Status=HIT
+CF-RAY=95b592b379c68c60-EWR
+alt-svc=h3=":443"; ma=86400</t>
+  </si>
+  <si>
+    <t>1694</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -63,12 +561,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray0625">
+        <bgColor indexed="13"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,8 +601,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,7 +919,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -387,48 +927,503 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="10" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.7109375"/>
+    <col min="2" max="2" customWidth="true" width="13.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625"/>
+    <col min="5" max="5" customWidth="true" width="13.5703125"/>
+    <col min="6" max="7" customWidth="true" width="19.85546875"/>
+    <col min="8" max="8" customWidth="true" width="23.140625"/>
+    <col min="9" max="10" customWidth="true" width="18.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s" s="11">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s" s="16">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s" s="17">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s" s="20">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s" s="22">
+        <v>19</v>
+      </c>
+      <c r="K14" t="s" s="0">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>